<commit_message>
Mission 3. Space part complete
</commit_message>
<xml_diff>
--- a/Assets/TEXT_2_0/voices.xlsx
+++ b/Assets/TEXT_2_0/voices.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -739,6 +739,18 @@
   </si>
   <si>
     <t>DX_M03_0000_wilhelm</t>
+  </si>
+  <si>
+    <t>DX_M03_1200_punisher</t>
+  </si>
+  <si>
+    <t>DX_M03_1210_hassler</t>
+  </si>
+  <si>
+    <t>0x9CAF4002</t>
+  </si>
+  <si>
+    <t>0x8ABAAD8D</t>
   </si>
 </sst>
 </file>
@@ -1814,9 +1826,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B56" sqref="A55:B56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2257,8 +2271,25 @@
         <v>221</v>
       </c>
     </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>241</v>
+      </c>
+      <c r="B55" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>242</v>
+      </c>
+      <c r="B56" t="s">
+        <v>244</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Mission 4 first half
</commit_message>
<xml_diff>
--- a/Assets/TEXT_2_0/voices.xlsx
+++ b/Assets/TEXT_2_0/voices.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="m02" sheetId="1" r:id="rId1"/>
     <sheet name="m03" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="m04" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="479">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -751,6 +751,708 @@
   </si>
   <si>
     <t>0x8ABAAD8D</t>
+  </si>
+  <si>
+    <t>DX_M04_0010_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0020_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0030_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0040_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0050_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0060_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0070_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0080_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0090_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0100_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0110_officer</t>
+  </si>
+  <si>
+    <t>DX_M04_0120_officer</t>
+  </si>
+  <si>
+    <t>DX_M04_0130_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0140_officer</t>
+  </si>
+  <si>
+    <t>DX_M04_0150_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0160_officer</t>
+  </si>
+  <si>
+    <t>DX_M04_0170_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0180_reichman</t>
+  </si>
+  <si>
+    <t>DX_M04_0190_reichman</t>
+  </si>
+  <si>
+    <t>DX_M04_0200_officer</t>
+  </si>
+  <si>
+    <t>DX_M04_0210_reichman</t>
+  </si>
+  <si>
+    <t>DX_M04_0220_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0230_alaric</t>
+  </si>
+  <si>
+    <t>DX_M04_0240_reichman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DX_M04_0250_officer </t>
+  </si>
+  <si>
+    <t>DX_M04_0260_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0270_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0280_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0290_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0300_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0310_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0320_alaric</t>
+  </si>
+  <si>
+    <t>DX_M04_0330_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0340_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0350_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0360_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0370_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0380_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0390_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0400_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0410_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0420_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0430_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0440_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0450_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0460_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0470_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0480_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0490_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0500_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0510_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0520_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0530_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0540_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0550_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0560_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0570_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0580_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0600_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0610_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0620_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0630_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0640_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0650_jacobo</t>
+  </si>
+  <si>
+    <t>DX_M04_0660_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0670_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0680_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0690_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0700_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0710_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0720_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0730_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0740_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0750_alaric</t>
+  </si>
+  <si>
+    <t>DX_M04_0760_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0770_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0780_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0790_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0800_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0810_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0820_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0830_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0840_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0850_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0860_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0870_alaric</t>
+  </si>
+  <si>
+    <t>DX_M04_0880_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0890_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0900_outpost</t>
+  </si>
+  <si>
+    <t>DX_M04_0910_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0920_outpost</t>
+  </si>
+  <si>
+    <t>DX_M04_0930_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0940_alaric</t>
+  </si>
+  <si>
+    <t>DX_M04_0950_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0960_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0970_alaric</t>
+  </si>
+  <si>
+    <t>DX_M04_0980_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_0990_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_0995_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_1000_alaric</t>
+  </si>
+  <si>
+    <t>DX_M04_1010_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_1020_hassler</t>
+  </si>
+  <si>
+    <t>DX_M04_1030_alaric</t>
+  </si>
+  <si>
+    <t>DX_M04_1040_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_1050_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_1060_alaric</t>
+  </si>
+  <si>
+    <t>0x9B02FF82</t>
+  </si>
+  <si>
+    <t>0xBCAAE1C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9B02B780 </t>
+  </si>
+  <si>
+    <t>0xBC72E7C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9B026F86 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xBC3AE5C2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xBC2EE4C8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xBB03DB8B </t>
+  </si>
+  <si>
+    <t>0xBDD6EAC8</t>
+  </si>
+  <si>
+    <t>0xBB16FA89</t>
+  </si>
+  <si>
+    <t>0xAAD01AC4</t>
+  </si>
+  <si>
+    <t>0x96D304C4</t>
+  </si>
+  <si>
+    <t>0x9B16B68A</t>
+  </si>
+  <si>
+    <t>0xAED578C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xA867ECC8 </t>
+  </si>
+  <si>
+    <t>0x86D76CC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9B16268E </t>
+  </si>
+  <si>
+    <t>0xA4056A06</t>
+  </si>
+  <si>
+    <t>0xA5056A02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xBDD110C8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xAD84D688 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9B797FCD </t>
+  </si>
+  <si>
+    <t>0x89A49807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xA8E4D689 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xB46A248F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xBB4A2185 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9F7C1DCD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9373FBCD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8772F1CD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xB27B6BC9 </t>
+  </si>
+  <si>
+    <t>0xA67A61C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9DB1930D </t>
+  </si>
+  <si>
+    <t>0x9B5EB48A</t>
+  </si>
+  <si>
+    <t>0xA27F03C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9B5E6C8C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8A7D17C9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9E7C1DC9 </t>
+  </si>
+  <si>
+    <t>0xBB5FD881</t>
+  </si>
+  <si>
+    <t>0x8672F1C9</t>
+  </si>
+  <si>
+    <t>0xBB92FF83</t>
+  </si>
+  <si>
+    <t>0xA11A61C0</t>
+  </si>
+  <si>
+    <t>0x9D197FC0</t>
+  </si>
+  <si>
+    <t>0x9B92B380</t>
+  </si>
+  <si>
+    <t>0xA51F03C0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9B926B86 </t>
+  </si>
+  <si>
+    <t>0x8D1D17C0</t>
+  </si>
+  <si>
+    <t>0x991C1DC0</t>
+  </si>
+  <si>
+    <t>0x9513FBC0</t>
+  </si>
+  <si>
+    <t>0x9B93DB8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xB41B6BC4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xA01A61C4 </t>
+  </si>
+  <si>
+    <t>0x9C197FC4</t>
+  </si>
+  <si>
+    <t>0x9B86B28A</t>
+  </si>
+  <si>
+    <t>0xA41F03C4</t>
+  </si>
+  <si>
+    <t>0xB01E09C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8C1D17C4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xB82B86C8 </t>
+  </si>
+  <si>
+    <t>0xBB87DE81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xB71B6BC8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x84F09EC8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9F197FC8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8B1875C8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x84749BC2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x84609AC8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xBBDA2585 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9B1C1DC8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xBBDBDD8B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8312F1C8 </t>
+  </si>
+  <si>
+    <t>0xB61B6BCC</t>
+  </si>
+  <si>
+    <t>0x9BCEF888</t>
+  </si>
+  <si>
+    <t>0x9E197FCC</t>
+  </si>
+  <si>
+    <t>0x9BCEB08A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xA61F03CC </t>
+  </si>
+  <si>
+    <t>0x8D79FC07</t>
+  </si>
+  <si>
+    <t>0x8E1D17CC</t>
+  </si>
+  <si>
+    <t>0x9BCE208E</t>
+  </si>
+  <si>
+    <t>0x9613FBCC</t>
+  </si>
+  <si>
+    <t>0x9BCFD880</t>
+  </si>
+  <si>
+    <t>0xB9FB6B8F</t>
+  </si>
+  <si>
+    <t>0x9A22F782</t>
+  </si>
+  <si>
+    <t>0x91F97F8F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9A22BF80 </t>
+  </si>
+  <si>
+    <t>0xA9FF038F</t>
+  </si>
+  <si>
+    <t>0x9A226786</t>
+  </si>
+  <si>
+    <t>0x81FD178F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x813E1807 </t>
+  </si>
+  <si>
+    <t>0xBA23D38B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8DF2F18F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x945A87C2 </t>
+  </si>
+  <si>
+    <t>0xACFA618B</t>
+  </si>
+  <si>
+    <t>0xBC5893C2</t>
+  </si>
+  <si>
+    <t>0x9A36BE8A</t>
+  </si>
+  <si>
+    <t>0x9563110D</t>
+  </si>
+  <si>
+    <t>0xBCFE098B</t>
+  </si>
+  <si>
+    <t>0x80FD178B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x953F1207 </t>
+  </si>
+  <si>
+    <t>0xBA37D281</t>
+  </si>
+  <si>
+    <t>0x8CF2F18B</t>
+  </si>
+  <si>
+    <t>0x8C76F481</t>
+  </si>
+  <si>
+    <t>0xA0FA8F09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8F03F582 </t>
+  </si>
+  <si>
+    <t>0x9979EB85</t>
+  </si>
+  <si>
+    <t>0xA0A68C03</t>
+  </si>
+  <si>
+    <t>0xAF036187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8F036586 </t>
+  </si>
+  <si>
+    <t>0xA0228909</t>
+  </si>
+  <si>
+    <t>DX_M04_0590_trent</t>
+  </si>
+  <si>
+    <t>0x9B87DA80</t>
+  </si>
+  <si>
+    <t>DX_M04_0000_jacobo</t>
+  </si>
+  <si>
+    <t>0xBCE2E3C2</t>
+  </si>
+  <si>
+    <t>DX_M04_1070_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M04_1080_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_1090_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M04_1100_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_1110_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_1130_trent</t>
+  </si>
+  <si>
+    <t>DX_M04_1140_hatcher</t>
+  </si>
+  <si>
+    <t>0xB51CA7C5</t>
+  </si>
+  <si>
+    <t>0xAF02D18B</t>
+  </si>
+  <si>
+    <t>0xAD124BC5</t>
+  </si>
+  <si>
+    <t>0xAF17F089</t>
+  </si>
+  <si>
+    <t>0x8F17F488</t>
+  </si>
+  <si>
+    <t>0x8F17BC8A</t>
+  </si>
+  <si>
+    <t>0x881FB9C1</t>
+  </si>
+  <si>
+    <t>DX_M04_0875_hassler</t>
+  </si>
+  <si>
+    <t>0x95781885</t>
+  </si>
+  <si>
+    <t>DX_M04_1120_hatcher</t>
+  </si>
+  <si>
+    <t>0xB019C5C1</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:D69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1828,9 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B56" sqref="A55:B56"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2295,12 +2995,959 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B117"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B10" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B12" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B13" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>257</v>
+      </c>
+      <c r="B14" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>259</v>
+      </c>
+      <c r="B16" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>260</v>
+      </c>
+      <c r="B17" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>262</v>
+      </c>
+      <c r="B19" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>263</v>
+      </c>
+      <c r="B20" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>264</v>
+      </c>
+      <c r="B21" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B22" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>266</v>
+      </c>
+      <c r="B23" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>267</v>
+      </c>
+      <c r="B24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>268</v>
+      </c>
+      <c r="B25" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>269</v>
+      </c>
+      <c r="B26" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>271</v>
+      </c>
+      <c r="B28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>272</v>
+      </c>
+      <c r="B29" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>273</v>
+      </c>
+      <c r="B30" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>274</v>
+      </c>
+      <c r="B31" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>275</v>
+      </c>
+      <c r="B32" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>276</v>
+      </c>
+      <c r="B33" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>277</v>
+      </c>
+      <c r="B34" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>278</v>
+      </c>
+      <c r="B35" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>279</v>
+      </c>
+      <c r="B36" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>280</v>
+      </c>
+      <c r="B37" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>281</v>
+      </c>
+      <c r="B38" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>282</v>
+      </c>
+      <c r="B39" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>283</v>
+      </c>
+      <c r="B40" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>284</v>
+      </c>
+      <c r="B41" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>285</v>
+      </c>
+      <c r="B42" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>286</v>
+      </c>
+      <c r="B43" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>287</v>
+      </c>
+      <c r="B44" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>288</v>
+      </c>
+      <c r="B45" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>289</v>
+      </c>
+      <c r="B46" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>290</v>
+      </c>
+      <c r="B47" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>291</v>
+      </c>
+      <c r="B48" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>292</v>
+      </c>
+      <c r="B49" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>293</v>
+      </c>
+      <c r="B50" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>294</v>
+      </c>
+      <c r="B51" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>295</v>
+      </c>
+      <c r="B52" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>296</v>
+      </c>
+      <c r="B53" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>297</v>
+      </c>
+      <c r="B54" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>298</v>
+      </c>
+      <c r="B55" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>299</v>
+      </c>
+      <c r="B56" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>300</v>
+      </c>
+      <c r="B57" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>301</v>
+      </c>
+      <c r="B58" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>302</v>
+      </c>
+      <c r="B59" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>457</v>
+      </c>
+      <c r="B60" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>303</v>
+      </c>
+      <c r="B61" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>304</v>
+      </c>
+      <c r="B62" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>305</v>
+      </c>
+      <c r="B63" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>306</v>
+      </c>
+      <c r="B64" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>307</v>
+      </c>
+      <c r="B65" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>308</v>
+      </c>
+      <c r="B66" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>309</v>
+      </c>
+      <c r="B67" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>310</v>
+      </c>
+      <c r="B68" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>311</v>
+      </c>
+      <c r="B69" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>312</v>
+      </c>
+      <c r="B70" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>313</v>
+      </c>
+      <c r="B71" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>314</v>
+      </c>
+      <c r="B72" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>315</v>
+      </c>
+      <c r="B73" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>316</v>
+      </c>
+      <c r="B74" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>317</v>
+      </c>
+      <c r="B75" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>318</v>
+      </c>
+      <c r="B76" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>319</v>
+      </c>
+      <c r="B77" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>320</v>
+      </c>
+      <c r="B78" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>321</v>
+      </c>
+      <c r="B79" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>322</v>
+      </c>
+      <c r="B80" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>323</v>
+      </c>
+      <c r="B81" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>324</v>
+      </c>
+      <c r="B82" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>325</v>
+      </c>
+      <c r="B83" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>326</v>
+      </c>
+      <c r="B84" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>327</v>
+      </c>
+      <c r="B85" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>328</v>
+      </c>
+      <c r="B86" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>329</v>
+      </c>
+      <c r="B87" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>330</v>
+      </c>
+      <c r="B88" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>475</v>
+      </c>
+      <c r="B89" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>331</v>
+      </c>
+      <c r="B90" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>332</v>
+      </c>
+      <c r="B91" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>333</v>
+      </c>
+      <c r="B92" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>334</v>
+      </c>
+      <c r="B93" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>335</v>
+      </c>
+      <c r="B94" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B95" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>337</v>
+      </c>
+      <c r="B96" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>338</v>
+      </c>
+      <c r="B97" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>339</v>
+      </c>
+      <c r="B98" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>340</v>
+      </c>
+      <c r="B99" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>341</v>
+      </c>
+      <c r="B100" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>342</v>
+      </c>
+      <c r="B101" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>343</v>
+      </c>
+      <c r="B102" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>344</v>
+      </c>
+      <c r="B103" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>345</v>
+      </c>
+      <c r="B104" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>346</v>
+      </c>
+      <c r="B105" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>347</v>
+      </c>
+      <c r="B106" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>348</v>
+      </c>
+      <c r="B107" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>349</v>
+      </c>
+      <c r="B108" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>350</v>
+      </c>
+      <c r="B109" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>461</v>
+      </c>
+      <c r="B110" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>462</v>
+      </c>
+      <c r="B111" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>463</v>
+      </c>
+      <c r="B112" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>464</v>
+      </c>
+      <c r="B113" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>465</v>
+      </c>
+      <c r="B114" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>477</v>
+      </c>
+      <c r="B115" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>466</v>
+      </c>
+      <c r="B116" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>467</v>
+      </c>
+      <c r="B117" t="s">
+        <v>474</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mission 4 Dialogs done
</commit_message>
<xml_diff>
--- a/Assets/TEXT_2_0/voices.xlsx
+++ b/Assets/TEXT_2_0/voices.xlsx
@@ -1143,9 +1143,6 @@
     <t xml:space="preserve">0xA8E4D689 </t>
   </si>
   <si>
-    <t xml:space="preserve">0xB46A248F </t>
-  </si>
-  <si>
     <t xml:space="preserve">0xBB4A2185 </t>
   </si>
   <si>
@@ -1453,6 +1450,9 @@
   </si>
   <si>
     <t>0xB019C5C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xB9D472C8 </t>
   </si>
 </sst>
 </file>
@@ -2998,7 +2998,7 @@
   <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3012,10 +3012,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B1" t="s">
         <v>459</v>
-      </c>
-      <c r="B1" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3215,7 +3215,7 @@
         <v>269</v>
       </c>
       <c r="B26" t="s">
-        <v>375</v>
+        <v>478</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -3223,7 +3223,7 @@
         <v>270</v>
       </c>
       <c r="B27" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -3231,7 +3231,7 @@
         <v>271</v>
       </c>
       <c r="B28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3239,7 +3239,7 @@
         <v>272</v>
       </c>
       <c r="B29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -3247,7 +3247,7 @@
         <v>273</v>
       </c>
       <c r="B30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3255,7 +3255,7 @@
         <v>274</v>
       </c>
       <c r="B31" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -3263,7 +3263,7 @@
         <v>275</v>
       </c>
       <c r="B32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3271,7 +3271,7 @@
         <v>276</v>
       </c>
       <c r="B33" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3279,7 +3279,7 @@
         <v>277</v>
       </c>
       <c r="B34" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3287,7 +3287,7 @@
         <v>278</v>
       </c>
       <c r="B35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3295,7 +3295,7 @@
         <v>279</v>
       </c>
       <c r="B36" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3303,7 +3303,7 @@
         <v>280</v>
       </c>
       <c r="B37" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3311,7 +3311,7 @@
         <v>281</v>
       </c>
       <c r="B38" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3319,7 +3319,7 @@
         <v>282</v>
       </c>
       <c r="B39" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -3327,7 +3327,7 @@
         <v>283</v>
       </c>
       <c r="B40" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -3335,7 +3335,7 @@
         <v>284</v>
       </c>
       <c r="B41" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -3343,7 +3343,7 @@
         <v>285</v>
       </c>
       <c r="B42" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -3351,7 +3351,7 @@
         <v>286</v>
       </c>
       <c r="B43" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3359,7 +3359,7 @@
         <v>287</v>
       </c>
       <c r="B44" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -3367,7 +3367,7 @@
         <v>288</v>
       </c>
       <c r="B45" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3375,7 +3375,7 @@
         <v>289</v>
       </c>
       <c r="B46" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3383,7 +3383,7 @@
         <v>290</v>
       </c>
       <c r="B47" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -3391,7 +3391,7 @@
         <v>291</v>
       </c>
       <c r="B48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3399,7 +3399,7 @@
         <v>292</v>
       </c>
       <c r="B49" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3407,7 +3407,7 @@
         <v>293</v>
       </c>
       <c r="B50" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3415,7 +3415,7 @@
         <v>294</v>
       </c>
       <c r="B51" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -3423,7 +3423,7 @@
         <v>295</v>
       </c>
       <c r="B52" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3431,7 +3431,7 @@
         <v>296</v>
       </c>
       <c r="B53" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3439,7 +3439,7 @@
         <v>297</v>
       </c>
       <c r="B54" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3447,7 +3447,7 @@
         <v>298</v>
       </c>
       <c r="B55" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3455,7 +3455,7 @@
         <v>299</v>
       </c>
       <c r="B56" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -3463,7 +3463,7 @@
         <v>300</v>
       </c>
       <c r="B57" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -3471,7 +3471,7 @@
         <v>301</v>
       </c>
       <c r="B58" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3479,15 +3479,15 @@
         <v>302</v>
       </c>
       <c r="B59" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
+        <v>456</v>
+      </c>
+      <c r="B60" t="s">
         <v>457</v>
-      </c>
-      <c r="B60" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -3495,7 +3495,7 @@
         <v>303</v>
       </c>
       <c r="B61" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -3503,7 +3503,7 @@
         <v>304</v>
       </c>
       <c r="B62" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -3511,7 +3511,7 @@
         <v>305</v>
       </c>
       <c r="B63" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -3519,7 +3519,7 @@
         <v>306</v>
       </c>
       <c r="B64" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -3527,7 +3527,7 @@
         <v>307</v>
       </c>
       <c r="B65" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -3535,7 +3535,7 @@
         <v>308</v>
       </c>
       <c r="B66" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -3543,7 +3543,7 @@
         <v>309</v>
       </c>
       <c r="B67" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -3551,7 +3551,7 @@
         <v>310</v>
       </c>
       <c r="B68" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -3559,7 +3559,7 @@
         <v>311</v>
       </c>
       <c r="B69" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -3567,7 +3567,7 @@
         <v>312</v>
       </c>
       <c r="B70" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -3575,7 +3575,7 @@
         <v>313</v>
       </c>
       <c r="B71" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -3583,7 +3583,7 @@
         <v>314</v>
       </c>
       <c r="B72" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -3591,7 +3591,7 @@
         <v>315</v>
       </c>
       <c r="B73" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -3599,7 +3599,7 @@
         <v>316</v>
       </c>
       <c r="B74" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -3607,7 +3607,7 @@
         <v>317</v>
       </c>
       <c r="B75" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -3615,7 +3615,7 @@
         <v>318</v>
       </c>
       <c r="B76" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -3623,7 +3623,7 @@
         <v>319</v>
       </c>
       <c r="B77" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -3631,7 +3631,7 @@
         <v>320</v>
       </c>
       <c r="B78" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -3639,7 +3639,7 @@
         <v>321</v>
       </c>
       <c r="B79" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -3647,7 +3647,7 @@
         <v>322</v>
       </c>
       <c r="B80" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -3655,7 +3655,7 @@
         <v>323</v>
       </c>
       <c r="B81" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -3663,7 +3663,7 @@
         <v>324</v>
       </c>
       <c r="B82" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -3671,7 +3671,7 @@
         <v>325</v>
       </c>
       <c r="B83" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -3679,7 +3679,7 @@
         <v>326</v>
       </c>
       <c r="B84" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -3687,7 +3687,7 @@
         <v>327</v>
       </c>
       <c r="B85" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -3695,7 +3695,7 @@
         <v>328</v>
       </c>
       <c r="B86" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -3703,7 +3703,7 @@
         <v>329</v>
       </c>
       <c r="B87" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -3711,15 +3711,15 @@
         <v>330</v>
       </c>
       <c r="B88" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
+        <v>474</v>
+      </c>
+      <c r="B89" t="s">
         <v>475</v>
-      </c>
-      <c r="B89" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -3727,7 +3727,7 @@
         <v>331</v>
       </c>
       <c r="B90" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -3735,7 +3735,7 @@
         <v>332</v>
       </c>
       <c r="B91" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -3743,7 +3743,7 @@
         <v>333</v>
       </c>
       <c r="B92" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -3751,7 +3751,7 @@
         <v>334</v>
       </c>
       <c r="B93" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -3759,7 +3759,7 @@
         <v>335</v>
       </c>
       <c r="B94" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -3767,7 +3767,7 @@
         <v>336</v>
       </c>
       <c r="B95" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -3775,7 +3775,7 @@
         <v>337</v>
       </c>
       <c r="B96" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -3783,7 +3783,7 @@
         <v>338</v>
       </c>
       <c r="B97" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -3791,7 +3791,7 @@
         <v>339</v>
       </c>
       <c r="B98" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -3799,7 +3799,7 @@
         <v>340</v>
       </c>
       <c r="B99" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -3807,7 +3807,7 @@
         <v>341</v>
       </c>
       <c r="B100" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -3815,7 +3815,7 @@
         <v>342</v>
       </c>
       <c r="B101" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -3823,7 +3823,7 @@
         <v>343</v>
       </c>
       <c r="B102" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -3831,7 +3831,7 @@
         <v>344</v>
       </c>
       <c r="B103" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -3839,7 +3839,7 @@
         <v>345</v>
       </c>
       <c r="B104" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -3847,7 +3847,7 @@
         <v>346</v>
       </c>
       <c r="B105" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -3855,7 +3855,7 @@
         <v>347</v>
       </c>
       <c r="B106" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -3863,7 +3863,7 @@
         <v>348</v>
       </c>
       <c r="B107" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -3871,7 +3871,7 @@
         <v>349</v>
       </c>
       <c r="B108" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -3879,71 +3879,71 @@
         <v>350</v>
       </c>
       <c r="B109" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B110" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B111" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B112" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B113" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B114" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
+        <v>476</v>
+      </c>
+      <c r="B115" t="s">
         <v>477</v>
-      </c>
-      <c r="B115" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B116" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B117" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mission 4 Done + ENG WITHOUT last cutscenes
</commit_message>
<xml_diff>
--- a/Assets/TEXT_2_0/voices.xlsx
+++ b/Assets/TEXT_2_0/voices.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="485">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -1453,6 +1453,24 @@
   </si>
   <si>
     <t xml:space="preserve">0xB9D472C8 </t>
+  </si>
+  <si>
+    <t>DX_M04_9100_officer</t>
+  </si>
+  <si>
+    <t>DX_M04_9200_cruiser</t>
+  </si>
+  <si>
+    <t>DX_M04_9300_hassler</t>
+  </si>
+  <si>
+    <t>0xBED5A686</t>
+  </si>
+  <si>
+    <t>0x9A544F40</t>
+  </si>
+  <si>
+    <t>0xB27FDD8B</t>
   </si>
 </sst>
 </file>
@@ -2995,10 +3013,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B117"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3946,6 +3964,30 @@
         <v>473</v>
       </c>
     </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>479</v>
+      </c>
+      <c r="B119" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>480</v>
+      </c>
+      <c r="B120" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>481</v>
+      </c>
+      <c r="B121" t="s">
+        <v>484</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>